<commit_message>
data provider working fine
</commit_message>
<xml_diff>
--- a/src/test/java/com/automation/utils/TodoApplication.xlsx
+++ b/src/test/java/com/automation/utils/TodoApplication.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14280" windowHeight="3960"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12630" windowHeight="6345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Development</t>
   </si>
@@ -53,6 +53,27 @@
   </si>
   <si>
     <t>TasksCompleted</t>
+  </si>
+  <si>
+    <t>TestCases</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>TC_06</t>
   </si>
 </sst>
 </file>
@@ -96,10 +117,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,85 +416,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A14" sqref="A14:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" customFormat="1">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" customFormat="1">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" customFormat="1">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" customFormat="1">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" customFormat="1">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" customFormat="1">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" customFormat="1">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" customFormat="1">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" customFormat="1">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="C15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
HTML reporting and added runner class to handle failed TC
</commit_message>
<xml_diff>
--- a/src/test/java/com/automation/utils/TodoApplication.xlsx
+++ b/src/test/java/com/automation/utils/TodoApplication.xlsx
@@ -7,17 +7,16 @@
     <workbookView xWindow="0" yWindow="2520" windowWidth="12630" windowHeight="6345"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A7:I25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="29">
   <si>
     <t>Development</t>
   </si>
@@ -74,13 +73,43 @@
   </si>
   <si>
     <t>TC_06</t>
+  </si>
+  <si>
+    <t>TC_07</t>
+  </si>
+  <si>
+    <t>TESTING</t>
+  </si>
+  <si>
+    <t>development</t>
+  </si>
+  <si>
+    <t>TC_08</t>
+  </si>
+  <si>
+    <t>test234689e2fvghdb</t>
+  </si>
+  <si>
+    <t>test2%^&amp;*%^#$@45723672%$#@(*(</t>
+  </si>
+  <si>
+    <t>TC_09</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>Analytics is the discovery, interpretation, and communication of meaningful patterns in data. Especially valuable in areas rich with recorded information, analytics relies on the simultaneous application of statistics, computer programming and operations research to quantify performance. Organizations may apply analytics to business data to describe, predict, and improve business performance. Specifically, areas within analytics include predictive analytics, prescriptive analytics, enterprise decision management,descriptive analytics,cognitive analytics, retail analytics, store assortment and stock-keeping unit optimization, marketing optimization and marketing mix modeling, web analytics, call analytics, speech analytics,sales force sizing and optimization, price and promotion modeling, predictive science, credit risk analysis, and fraud analytics. Since analytics can require extensive computation (see big data), the algorithms and software used for analytics harness the most current methods in computer science, statistics, and mathematics.[1]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +124,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,16 +150,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,16 +461,481 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A15"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="390">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" ref="B7:B50" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(10,99)</f>
+        <v>GL46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>CJ48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>GR30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>OV84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>JM58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>MO58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>UI18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>MG62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>JK33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>BG72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>BN91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>QJ57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LP93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>BS84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>FV37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>BA27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>BT81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>ZU45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>TA36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>CH41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>EX82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>BC45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LE85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>TD68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>VB70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>GI31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LX96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>UJ41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>WX93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>WV81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>PJ50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>EH68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>TS48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>FE86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>HZ29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>WF76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>KU43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>BM82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>WD86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>PI53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>OM57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LF52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>SA78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LX84</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -484,7 +994,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" customFormat="1">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -493,7 +1003,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" customFormat="1">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -502,7 +1012,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" customFormat="1">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -511,7 +1021,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" customFormat="1">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -520,7 +1030,7 @@
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" customFormat="1">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -529,7 +1039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" customFormat="1">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -538,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" customFormat="1">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -547,7 +1057,7 @@
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" customFormat="1">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -556,7 +1066,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" customFormat="1">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -566,31 +1076,6 @@
       <c r="C15" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>